<commit_message>
Big Data - T7 Completed
</commit_message>
<xml_diff>
--- a/BigData/T7/original_Describe.xlsx
+++ b/BigData/T7/original_Describe.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Game Played</t>
   </si>
   <si>
     <t>Wins</t>
+  </si>
+  <si>
+    <t>Losses</t>
   </si>
   <si>
     <t>WIN %</t>
@@ -470,13 +473,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,10 +555,13 @@
       <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:27">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>30</v>
@@ -632,10 +638,13 @@
       <c r="Z2">
         <v>30</v>
       </c>
+      <c r="AA2">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:27">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>82</v>
@@ -644,553 +653,574 @@
         <v>41</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>41</v>
       </c>
       <c r="E3">
-        <v>48.28333333333332</v>
+        <v>0.4999666666666667</v>
       </c>
       <c r="F3">
-        <v>106.3366666666667</v>
+        <v>48.32000000000001</v>
       </c>
       <c r="G3">
-        <v>39.60666666666667</v>
+        <v>111.2033333333334</v>
       </c>
       <c r="H3">
-        <v>86.06333333333335</v>
+        <v>41.07333333333334</v>
       </c>
       <c r="I3">
-        <v>46.02666666666667</v>
+        <v>89.21333333333334</v>
       </c>
       <c r="J3">
-        <v>10.48666666666667</v>
+        <v>46.04666666666666</v>
       </c>
       <c r="K3">
-        <v>28.99666666666667</v>
+        <v>11.36</v>
       </c>
       <c r="L3">
-        <v>36.17333333333333</v>
+        <v>32.00666666666667</v>
       </c>
       <c r="M3">
-        <v>16.61333333333333</v>
+        <v>35.55</v>
       </c>
       <c r="N3">
-        <v>21.67333333333334</v>
+        <v>17.67666666666667</v>
       </c>
       <c r="O3">
-        <v>76.75000000000001</v>
+        <v>23.07333333333333</v>
       </c>
       <c r="P3">
-        <v>9.716666666666667</v>
+        <v>76.69666666666669</v>
       </c>
       <c r="Q3">
-        <v>33.80333333333333</v>
+        <v>10.34666666666667</v>
       </c>
       <c r="R3">
-        <v>43.51666666666667</v>
+        <v>34.82333333333334</v>
       </c>
       <c r="S3">
-        <v>23.24000000000001</v>
+        <v>45.17</v>
       </c>
       <c r="T3">
-        <v>14.26</v>
+        <v>24.57999999999999</v>
       </c>
       <c r="U3">
-        <v>7.713333333333333</v>
+        <v>14.07666666666667</v>
       </c>
       <c r="V3">
-        <v>4.803333333333334</v>
+        <v>7.623333333333334</v>
       </c>
       <c r="W3">
-        <v>4.816666666666667</v>
+        <v>4.946666666666667</v>
       </c>
       <c r="X3">
-        <v>19.85666666666667</v>
+        <v>4.953333333333333</v>
       </c>
       <c r="Y3">
-        <v>19.86</v>
+        <v>20.90333333333333</v>
       </c>
       <c r="Z3">
-        <v>0.006666666666666228</v>
+        <v>20.89333333333333</v>
+      </c>
+      <c r="AA3">
+        <v>0.01333333333333305</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:27">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>12.22208289715086</v>
+        <v>12.02870130863734</v>
       </c>
       <c r="D4">
-        <v>0.1490803995072504</v>
+        <v>12.02870130863734</v>
       </c>
       <c r="E4">
-        <v>0.1641768040513199</v>
+        <v>0.1467069524087303</v>
       </c>
       <c r="F4">
-        <v>3.800860459144095</v>
+        <v>0.1584406774659267</v>
       </c>
       <c r="G4">
-        <v>1.393317384278734</v>
+        <v>4.093180479380504</v>
       </c>
       <c r="H4">
-        <v>1.552191628174405</v>
+        <v>1.672069404048176</v>
       </c>
       <c r="I4">
-        <v>1.504460800037865</v>
+        <v>2.110194194909529</v>
       </c>
       <c r="J4">
-        <v>1.505102432837491</v>
+        <v>1.323457679672855</v>
       </c>
       <c r="K4">
-        <v>4.020506344276528</v>
+        <v>1.509190237317282</v>
       </c>
       <c r="L4">
-        <v>1.128298485004907</v>
+        <v>4.300676236588152</v>
       </c>
       <c r="M4">
-        <v>1.742715545137636</v>
+        <v>1.53212721178871</v>
       </c>
       <c r="N4">
-        <v>2.293458964749208</v>
+        <v>1.693534018336913</v>
       </c>
       <c r="O4">
-        <v>2.398814362310595</v>
+        <v>2.172545516896828</v>
       </c>
       <c r="P4">
-        <v>0.9381137837513996</v>
+        <v>3.219604102170429</v>
       </c>
       <c r="Q4">
-        <v>1.381024940056287</v>
+        <v>0.9877642233445895</v>
       </c>
       <c r="R4">
-        <v>1.73127087729642</v>
+        <v>1.805295530937522</v>
       </c>
       <c r="S4">
-        <v>1.956527536223296</v>
+        <v>2.110915800604415</v>
       </c>
       <c r="T4">
-        <v>1.024055494185942</v>
+        <v>2.086971076910763</v>
       </c>
       <c r="U4">
-        <v>0.6729929719022965</v>
+        <v>1.024083554421602</v>
       </c>
       <c r="V4">
-        <v>0.8040772536796806</v>
+        <v>0.8402312215974402</v>
       </c>
       <c r="W4">
-        <v>0.5153394149913998</v>
+        <v>0.730013383596414</v>
       </c>
       <c r="X4">
-        <v>1.400660763608606</v>
+        <v>0.6129259016549555</v>
       </c>
       <c r="Y4">
-        <v>1.196719654319458</v>
+        <v>1.341507986618388</v>
       </c>
       <c r="Z4">
-        <v>4.456141313098009</v>
+        <v>1.268975512204515</v>
+      </c>
+      <c r="AA4">
+        <v>4.887615124904517</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:27">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>82</v>
       </c>
       <c r="C5">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D5">
-        <v>0.256</v>
+        <v>22</v>
       </c>
       <c r="E5">
+        <v>0.207</v>
+      </c>
+      <c r="F5">
         <v>48.1</v>
       </c>
-      <c r="F5">
-        <v>98.8</v>
-      </c>
       <c r="G5">
-        <v>36.7</v>
+        <v>103.5</v>
       </c>
       <c r="H5">
-        <v>82.8</v>
+        <v>38</v>
       </c>
       <c r="I5">
-        <v>43.5</v>
+        <v>84.40000000000001</v>
       </c>
       <c r="J5">
-        <v>8</v>
+        <v>43.3</v>
       </c>
       <c r="K5">
-        <v>22.5</v>
+        <v>9.1</v>
       </c>
       <c r="L5">
-        <v>33.4</v>
+        <v>25.3</v>
       </c>
       <c r="M5">
-        <v>12.3</v>
+        <v>32.9</v>
       </c>
       <c r="N5">
-        <v>16.7</v>
+        <v>15</v>
       </c>
       <c r="O5">
-        <v>71.40000000000001</v>
+        <v>19.2</v>
       </c>
       <c r="P5">
-        <v>8.1</v>
+        <v>69.5</v>
       </c>
       <c r="Q5">
-        <v>31</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="R5">
-        <v>39.8</v>
+        <v>31.3</v>
       </c>
       <c r="S5">
-        <v>19.5</v>
+        <v>40.4</v>
       </c>
       <c r="T5">
-        <v>12.3</v>
+        <v>20.1</v>
       </c>
       <c r="U5">
-        <v>6.2</v>
+        <v>12.1</v>
       </c>
       <c r="V5">
-        <v>3.5</v>
+        <v>6.1</v>
       </c>
       <c r="W5">
-        <v>3.7</v>
+        <v>2.4</v>
       </c>
       <c r="X5">
-        <v>17.2</v>
+        <v>3.6</v>
       </c>
       <c r="Y5">
-        <v>17.3</v>
+        <v>18.1</v>
       </c>
       <c r="Z5">
-        <v>-9.4</v>
+        <v>18.7</v>
+      </c>
+      <c r="AA5">
+        <v>-9.6</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:27">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>82</v>
       </c>
       <c r="C6">
-        <v>28.25</v>
+        <v>33</v>
       </c>
       <c r="D6">
-        <v>0.3442500000000001</v>
+        <v>32.25</v>
       </c>
       <c r="E6">
-        <v>48.125</v>
+        <v>0.402</v>
       </c>
       <c r="F6">
-        <v>103.5</v>
+        <v>48.2</v>
       </c>
       <c r="G6">
-        <v>38.7</v>
+        <v>107.625</v>
       </c>
       <c r="H6">
-        <v>85.32499999999999</v>
+        <v>39.875</v>
       </c>
       <c r="I6">
+        <v>87.67499999999998</v>
+      </c>
+      <c r="J6">
         <v>45</v>
       </c>
-      <c r="J6">
-        <v>9.350000000000001</v>
-      </c>
       <c r="K6">
-        <v>26.575</v>
+        <v>10.15</v>
       </c>
       <c r="L6">
-        <v>35.425</v>
+        <v>29.35</v>
       </c>
       <c r="M6">
-        <v>15.575</v>
+        <v>34.8</v>
       </c>
       <c r="N6">
-        <v>20.225</v>
+        <v>16.325</v>
       </c>
       <c r="O6">
-        <v>75.27500000000001</v>
+        <v>21.25</v>
       </c>
       <c r="P6">
-        <v>9.025</v>
+        <v>74.825</v>
       </c>
       <c r="Q6">
-        <v>32.875</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="R6">
-        <v>42.15000000000001</v>
+        <v>33.75</v>
       </c>
       <c r="S6">
-        <v>22.225</v>
+        <v>43.97499999999999</v>
       </c>
       <c r="T6">
-        <v>13.55</v>
+        <v>23.4</v>
       </c>
       <c r="U6">
-        <v>7.425000000000001</v>
+        <v>13.425</v>
       </c>
       <c r="V6">
-        <v>4.225000000000001</v>
+        <v>6.824999999999999</v>
       </c>
       <c r="W6">
+        <v>4.625</v>
+      </c>
+      <c r="X6">
         <v>4.525</v>
       </c>
-      <c r="X6">
-        <v>19.125</v>
-      </c>
       <c r="Y6">
-        <v>19.125</v>
+        <v>20.15</v>
       </c>
       <c r="Z6">
-        <v>-3.45</v>
+        <v>20.025</v>
+      </c>
+      <c r="AA6">
+        <v>-1.65</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:27">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>82</v>
       </c>
       <c r="C7">
-        <v>44</v>
+        <v>41.5</v>
       </c>
       <c r="D7">
-        <v>0.537</v>
+        <v>40.5</v>
       </c>
       <c r="E7">
-        <v>48.25</v>
+        <v>0.506</v>
       </c>
       <c r="F7">
-        <v>106.05</v>
+        <v>48.3</v>
       </c>
       <c r="G7">
-        <v>39.2</v>
+        <v>112</v>
       </c>
       <c r="H7">
-        <v>86.09999999999999</v>
+        <v>41.34999999999999</v>
       </c>
       <c r="I7">
-        <v>45.85</v>
+        <v>89.09999999999999</v>
       </c>
       <c r="J7">
-        <v>10.5</v>
+        <v>46.15</v>
       </c>
       <c r="K7">
-        <v>29</v>
+        <v>11.3</v>
       </c>
       <c r="L7">
-        <v>36</v>
+        <v>31.75</v>
       </c>
       <c r="M7">
-        <v>16.65</v>
+        <v>35.25</v>
       </c>
       <c r="N7">
-        <v>21.3</v>
+        <v>17.7</v>
       </c>
       <c r="O7">
-        <v>77.2</v>
+        <v>23.15</v>
       </c>
       <c r="P7">
-        <v>9.649999999999999</v>
+        <v>77.15000000000001</v>
       </c>
       <c r="Q7">
-        <v>33.8</v>
+        <v>10.15</v>
       </c>
       <c r="R7">
-        <v>43.8</v>
+        <v>34.90000000000001</v>
       </c>
       <c r="S7">
-        <v>22.8</v>
+        <v>45.34999999999999</v>
       </c>
       <c r="T7">
-        <v>14.2</v>
+        <v>24.55</v>
       </c>
       <c r="U7">
-        <v>7.7</v>
+        <v>14</v>
       </c>
       <c r="V7">
-        <v>4.8</v>
+        <v>7.55</v>
       </c>
       <c r="W7">
-        <v>4.75</v>
+        <v>5.05</v>
       </c>
       <c r="X7">
-        <v>19.6</v>
+        <v>5.05</v>
       </c>
       <c r="Y7">
-        <v>19.95</v>
+        <v>20.9</v>
       </c>
       <c r="Z7">
-        <v>0.55</v>
+        <v>20.75</v>
+      </c>
+      <c r="AA7">
+        <v>-0.15</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:27">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>82</v>
       </c>
       <c r="C8">
-        <v>48</v>
+        <v>49.75</v>
       </c>
       <c r="D8">
-        <v>0.585</v>
+        <v>49</v>
       </c>
       <c r="E8">
+        <v>0.607</v>
+      </c>
+      <c r="F8">
         <v>48.4</v>
       </c>
-      <c r="F8">
-        <v>109.375</v>
-      </c>
       <c r="G8">
-        <v>40.7</v>
+        <v>114.35</v>
       </c>
       <c r="H8">
-        <v>86.97499999999999</v>
+        <v>42.275</v>
       </c>
       <c r="I8">
-        <v>47.175</v>
+        <v>90.5</v>
       </c>
       <c r="J8">
-        <v>11.275</v>
+        <v>47.075</v>
       </c>
       <c r="K8">
-        <v>30.825</v>
+        <v>12.325</v>
       </c>
       <c r="L8">
-        <v>36.9</v>
+        <v>34.3</v>
       </c>
       <c r="M8">
-        <v>17.375</v>
+        <v>35.9</v>
       </c>
       <c r="N8">
-        <v>23.3</v>
+        <v>18.7</v>
       </c>
       <c r="O8">
-        <v>78.25</v>
+        <v>24.2</v>
       </c>
       <c r="P8">
-        <v>10.275</v>
+        <v>79.17500000000001</v>
       </c>
       <c r="Q8">
-        <v>34.95</v>
+        <v>11.075</v>
       </c>
       <c r="R8">
-        <v>44.475</v>
+        <v>35.75</v>
       </c>
       <c r="S8">
-        <v>23.7</v>
+        <v>46.4</v>
       </c>
       <c r="T8">
-        <v>14.975</v>
+        <v>26</v>
       </c>
       <c r="U8">
-        <v>8</v>
+        <v>14.65</v>
       </c>
       <c r="V8">
-        <v>5.1</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="W8">
-        <v>5.1</v>
+        <v>5.375000000000001</v>
       </c>
       <c r="X8">
-        <v>20.575</v>
+        <v>5.375000000000001</v>
       </c>
       <c r="Y8">
-        <v>20.5</v>
+        <v>21.475</v>
       </c>
       <c r="Z8">
-        <v>2.825</v>
+        <v>21.775</v>
+      </c>
+      <c r="AA8">
+        <v>3.85</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:27">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>82</v>
       </c>
       <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9">
         <v>65</v>
       </c>
-      <c r="D9">
-        <v>0.7929999999999999</v>
-      </c>
       <c r="E9">
+        <v>0.732</v>
+      </c>
+      <c r="F9">
         <v>48.7</v>
       </c>
-      <c r="F9">
-        <v>113.5</v>
-      </c>
       <c r="G9">
-        <v>42.8</v>
+        <v>118.1</v>
       </c>
       <c r="H9">
-        <v>88.8</v>
+        <v>44</v>
       </c>
       <c r="I9">
-        <v>50.3</v>
+        <v>94</v>
       </c>
       <c r="J9">
-        <v>15.3</v>
+        <v>49.1</v>
       </c>
       <c r="K9">
-        <v>42.3</v>
+        <v>16.1</v>
       </c>
       <c r="L9">
-        <v>39.1</v>
+        <v>45.4</v>
       </c>
       <c r="M9">
-        <v>20.2</v>
+        <v>39.2</v>
       </c>
       <c r="N9">
-        <v>27</v>
+        <v>22.6</v>
       </c>
       <c r="O9">
-        <v>81.5</v>
+        <v>28.5</v>
       </c>
       <c r="P9">
-        <v>12.5</v>
+        <v>81.90000000000001</v>
       </c>
       <c r="Q9">
-        <v>36.5</v>
+        <v>12.6</v>
       </c>
       <c r="R9">
-        <v>47.4</v>
+        <v>40.4</v>
       </c>
       <c r="S9">
-        <v>29.3</v>
+        <v>49.7</v>
       </c>
       <c r="T9">
-        <v>16.5</v>
+        <v>29.4</v>
       </c>
       <c r="U9">
-        <v>9.1</v>
+        <v>17</v>
       </c>
       <c r="V9">
-        <v>7.5</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="W9">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="X9">
-        <v>23.2</v>
+        <v>6.1</v>
       </c>
       <c r="Y9">
-        <v>22.4</v>
+        <v>23.6</v>
       </c>
       <c r="Z9">
-        <v>8.5</v>
+        <v>24</v>
+      </c>
+      <c r="AA9">
+        <v>8.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>